<commit_message>
updated parts list to match PCB. Added tactile SPDT details fo boot mode
</commit_message>
<xml_diff>
--- a/Altium Part to Make.xlsx
+++ b/Altium Part to Make.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Engineering work\blackmagic\L1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87130C6-9567-4638-84B1-AB61B9AE25C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FECCCD-C516-4BEF-9E4C-6D35EC324059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57600" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{81953BA9-CB8D-4A4B-B37A-041E33955A54}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>RP2040</t>
   </si>
@@ -118,9 +118,6 @@
     <t>DG2735ADN-T1-GE4</t>
   </si>
   <si>
-    <t>DPDT IC switch</t>
-  </si>
-  <si>
     <t>27PSO 0.3mm Molex conn</t>
   </si>
   <si>
@@ -170,6 +167,72 @@
   </si>
   <si>
     <t>Octocoupler</t>
+  </si>
+  <si>
+    <t>KJ01EXT</t>
+  </si>
+  <si>
+    <t>Slide SPDT</t>
+  </si>
+  <si>
+    <t>SS312SAH4-R</t>
+  </si>
+  <si>
+    <t>Slide SPDT backup</t>
+  </si>
+  <si>
+    <t>NS5A4684SMNTBG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dual IC SPDT </t>
+  </si>
+  <si>
+    <t>B39162B9415K610</t>
+  </si>
+  <si>
+    <t>GPS DAW filter</t>
+  </si>
+  <si>
+    <t>APG0603CGC-TT</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>2305018-2</t>
+  </si>
+  <si>
+    <t>BMI090L</t>
+  </si>
+  <si>
+    <t>Backups</t>
+  </si>
+  <si>
+    <t>HP0315AFKP2-R</t>
+  </si>
+  <si>
+    <t>Tactile SPST</t>
+  </si>
+  <si>
+    <t>TS3A24159YZPR</t>
+  </si>
+  <si>
+    <t>IC SPDT</t>
+  </si>
+  <si>
+    <t>SPDT IC switch</t>
+  </si>
+  <si>
+    <t>SS-5GL</t>
+  </si>
+  <si>
+    <t>SPDT limit switch</t>
+  </si>
+  <si>
+    <t>1-2307813-0</t>
+  </si>
+  <si>
+    <t>2mm 10pos socket for xbee</t>
   </si>
 </sst>
 </file>
@@ -193,12 +256,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -222,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -240,6 +309,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA0D536-DA6B-42C0-8A72-A9C87B3276BA}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,16 +642,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -589,6 +661,9 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -597,6 +672,9 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -605,6 +683,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -613,6 +694,9 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -621,21 +705,30 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,6 +738,9 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -653,6 +749,9 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -661,96 +760,264 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
+      <c r="A14" s="4">
+        <v>5025982793</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>5025982793</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A27:D27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
first 4 line items added to Altium Library
</commit_message>
<xml_diff>
--- a/Altium Part to Make.xlsx
+++ b/Altium Part to Make.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Engineering work\blackmagic\L1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FECCCD-C516-4BEF-9E4C-6D35EC324059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968A6314-D832-4BD3-8B7B-2B2C014D9582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57600" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{81953BA9-CB8D-4A4B-B37A-041E33955A54}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>RP2040</t>
   </si>
@@ -629,7 +630,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,6 +665,9 @@
       <c r="C2" t="s">
         <v>53</v>
       </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -675,6 +679,9 @@
       <c r="C3" t="s">
         <v>53</v>
       </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -686,6 +693,9 @@
       <c r="C4" t="s">
         <v>53</v>
       </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -695,6 +705,9 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated to reflect made altium parts.
</commit_message>
<xml_diff>
--- a/Altium Part to Make.xlsx
+++ b/Altium Part to Make.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Engineering work\blackmagic\L1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968A6314-D832-4BD3-8B7B-2B2C014D9582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512A4BB2-9B53-40E4-8389-EDE7C09F8512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57600" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{81953BA9-CB8D-4A4B-B37A-041E33955A54}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
   <si>
     <t>RP2040</t>
   </si>
@@ -191,9 +190,6 @@
     <t>B39162B9415K610</t>
   </si>
   <si>
-    <t>GPS DAW filter</t>
-  </si>
-  <si>
     <t>APG0603CGC-TT</t>
   </si>
   <si>
@@ -234,6 +230,18 @@
   </si>
   <si>
     <t>2mm 10pos socket for xbee</t>
+  </si>
+  <si>
+    <t>use standard 0402 inductor size</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>GPS SAW filter</t>
   </si>
 </sst>
 </file>
@@ -292,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -310,6 +318,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -627,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA0D536-DA6B-42C0-8A72-A9C87B3276BA}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,9 +648,10 @@
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -654,8 +664,11 @@
       <c r="D1" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,13 +676,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -677,13 +690,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -691,13 +704,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -705,13 +718,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -719,10 +732,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -730,10 +746,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -741,10 +760,13 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -752,10 +774,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -763,10 +788,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -774,10 +802,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -785,10 +816,13 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -796,10 +830,13 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>5025982793</v>
       </c>
@@ -807,10 +844,13 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -818,10 +858,16 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -829,7 +875,10 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,7 +889,10 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,7 +903,10 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -862,18 +917,24 @@
         <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,7 +945,10 @@
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,7 +959,10 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,7 +973,10 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,62 +984,74 @@
         <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
         <v>64</v>
       </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="A27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,7 +1062,7 @@
         <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -991,18 +1073,18 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
         <v>59</v>
       </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1010,21 +1092,21 @@
         <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
         <v>62</v>
       </c>
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>